<commit_message>
Added more Tips including SQL Server
</commit_message>
<xml_diff>
--- a/Tips/2024.04컴구매분석.xlsx
+++ b/Tips/2024.04컴구매분석.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocuments\Documents\백종근\백종근\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepositories\CodeSnippet\Tips\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D8253D-49BB-4C1B-8D29-070332E80620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMD 5세대" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,28 @@
     <definedName name="productName" localSheetId="1">'AMD 4세대'!$B$6</definedName>
     <definedName name="productName" localSheetId="0">'AMD 5세대'!$B$7</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>CPU</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -43,10 +55,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>AMD 75000f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>메인보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -143,10 +151,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>중고구매 추가#1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>중고구매 추가-ITX</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -159,10 +163,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>중고구매 추가-13500</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://youtu.be/PthqQUBEolI?si=cRHTeYN5kIoAs50q</t>
   </si>
   <si>
@@ -171,10 +171,6 @@
   </si>
   <si>
     <t>용량감소</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중고구매 추가#2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -203,13 +199,48 @@
   </si>
   <si>
     <t>케이스 - 리안리 LANCOOL 216 (블랙)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMD 7600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중고구매 추가#1
+(5600, 6700xt, A320m)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중고구매 추가#0
+(5800X, 64GB RAM)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>개별 구매
+(8600G, T500)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8600G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T500</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDR5 64G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P 700W</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -346,7 +377,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -451,6 +482,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -458,7 +495,15 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -733,52 +778,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.375" customWidth="1"/>
     <col min="3" max="3" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
     <col min="6" max="6" width="10.875" customWidth="1"/>
     <col min="7" max="7" width="4.25" customWidth="1"/>
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.25" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.25" customWidth="1"/>
-    <col min="15" max="15" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.25" customWidth="1"/>
+    <col min="18" max="18" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34.5" customHeight="1">
+    <row r="1" spans="1:19" ht="34.5" customHeight="1">
       <c r="C1" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="7"/>
       <c r="G1" s="15"/>
       <c r="H1" s="27" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I1" s="27"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="29"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="J1" s="15"/>
+      <c r="K1" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="27"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="31"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="29"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -786,55 +841,63 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="17"/>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="9"/>
+      <c r="Q2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1">
-        <v>215100</v>
+        <v>227430</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="2">
         <f>$C3*D3</f>
-        <v>215100</v>
+        <v>227430</v>
       </c>
       <c r="F3" s="2">
         <v>190000</v>
@@ -845,17 +908,17 @@
       </c>
       <c r="I3" s="2">
         <f>$C3*H3</f>
-        <v>215100</v>
-      </c>
-      <c r="J3" s="5"/>
+        <v>227430</v>
+      </c>
+      <c r="J3" s="16"/>
       <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
         <f>$C3*K3</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="10"/>
+        <v>227430</v>
+      </c>
+      <c r="M3" s="5"/>
       <c r="N3">
         <v>0</v>
       </c>
@@ -863,13 +926,22 @@
         <f>$C3*N3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="10"/>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <f>$C3*Q3</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="10"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>24850</v>
@@ -881,7 +953,10 @@
         <f t="shared" ref="E4:E14" si="0">$C4*D4</f>
         <v>24850</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <f>E4</f>
+        <v>24850</v>
+      </c>
       <c r="G4" s="16"/>
       <c r="H4">
         <v>1</v>
@@ -890,29 +965,38 @@
         <f t="shared" ref="I4:I14" si="1">$C4*H4</f>
         <v>24850</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="16"/>
       <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <f t="shared" ref="L4:L13" si="2">$C4*K4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L14" si="2">$C4*K4</f>
+        <v>24850</v>
+      </c>
+      <c r="M4" s="5"/>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O14" si="3">$C4*N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <f t="shared" ref="O4:O13" si="3">$C4*N4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R14" si="4">$C4*Q4</f>
+        <v>24850</v>
+      </c>
+      <c r="S4" s="10"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>158600</v>
@@ -924,24 +1008,27 @@
         <f t="shared" si="0"/>
         <v>158600</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F11" si="5">E5</f>
+        <v>158600</v>
+      </c>
       <c r="G5" s="16"/>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="5"/>
+        <v>158600</v>
+      </c>
+      <c r="J5" s="16"/>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="5"/>
       <c r="N5">
         <v>0</v>
       </c>
@@ -949,10 +1036,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="10"/>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="4"/>
+        <v>158600</v>
+      </c>
+      <c r="S5" s="10"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <v>181330</v>
@@ -964,31 +1060,50 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="G6" s="16"/>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="2"/>
         <v>181330</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="M6" s="5"/>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="10"/>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>56610</v>
@@ -1000,38 +1115,50 @@
         <f t="shared" si="0"/>
         <v>113220</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <f t="shared" si="5"/>
+        <v>113220</v>
+      </c>
       <c r="G7" s="16"/>
       <c r="H7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
+        <v>56610</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
         <v>226440</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="5"/>
       <c r="N7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="3"/>
-        <v>113220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="1">
         <v>137500</v>
@@ -1043,38 +1170,50 @@
         <f t="shared" si="0"/>
         <v>137500</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <f t="shared" si="5"/>
+        <v>137500</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
+        <v>68750</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="2"/>
         <v>275000</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="5"/>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="3"/>
-        <v>137500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
         <v>79600</v>
@@ -1086,7 +1225,10 @@
         <f t="shared" si="0"/>
         <v>79600</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <f t="shared" si="5"/>
+        <v>79600</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9">
         <v>1</v>
@@ -1095,15 +1237,15 @@
         <f t="shared" si="1"/>
         <v>79600</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="16"/>
       <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="10"/>
+        <v>79600</v>
+      </c>
+      <c r="M9" s="5"/>
       <c r="N9">
         <v>0</v>
       </c>
@@ -1111,13 +1253,22 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="10"/>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>51000</v>
@@ -1129,7 +1280,10 @@
         <f t="shared" si="0"/>
         <v>51000</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <f t="shared" si="5"/>
+        <v>51000</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10">
         <v>1</v>
@@ -1138,15 +1292,15 @@
         <f t="shared" si="1"/>
         <v>51000</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="16"/>
       <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="10"/>
+        <v>51000</v>
+      </c>
+      <c r="M10" s="5"/>
       <c r="N10">
         <v>0</v>
       </c>
@@ -1154,13 +1308,22 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="10"/>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="4"/>
+        <v>51000</v>
+      </c>
+      <c r="S10" s="10"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
         <v>11300</v>
@@ -1172,24 +1335,27 @@
         <f t="shared" si="0"/>
         <v>22600</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <f t="shared" si="5"/>
+        <v>22600</v>
+      </c>
       <c r="G11" s="16"/>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
         <v>22600</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="10"/>
+      <c r="M11" s="5"/>
       <c r="N11">
         <v>0</v>
       </c>
@@ -1197,13 +1363,22 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="10"/>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="4"/>
+        <v>22600</v>
+      </c>
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>258000</v>
@@ -1215,24 +1390,26 @@
         <f t="shared" si="0"/>
         <v>258000</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2">
+        <v>110000</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
         <v>258000</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="10"/>
+      <c r="M12" s="5"/>
       <c r="N12">
         <v>0</v>
       </c>
@@ -1240,8 +1417,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="10"/>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="10"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1252,18 +1438,24 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="L13" s="1">
+      <c r="J13" s="16"/>
+      <c r="L13" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M13" s="10"/>
+      <c r="M13" s="4"/>
       <c r="O13" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="10"/>
+      <c r="R13" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="10"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1274,97 +1466,174 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="L14" s="1">
-        <f>SUM(L3:L13)</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="11"/>
+      <c r="J14" s="17"/>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="5"/>
       <c r="O14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <f>SUM(O3:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="R14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2">
         <f>SUM(E3:E14)</f>
-        <v>1060470</v>
+        <v>1072800</v>
       </c>
       <c r="F15" s="2">
         <f>SUM(F3:F14)</f>
-        <v>190000</v>
+        <v>887370</v>
       </c>
       <c r="G15" s="16"/>
       <c r="I15" s="2">
         <f>SUM(I3:I14)</f>
-        <v>1333920</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1150000</v>
-      </c>
-      <c r="M15" s="10"/>
-      <c r="O15" s="1">
+        <v>666840</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="L15" s="2">
+        <f>SUM(L3:L14)</f>
+        <v>1346250</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="2">
         <f>SUM(O3:O14)</f>
-        <v>250720</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="G16" s="17"/>
-      <c r="J16" s="4"/>
-      <c r="L16" s="18">
-        <f>SUM(L14:L15)</f>
-        <v>1150000</v>
-      </c>
-      <c r="M16" s="11"/>
-      <c r="N16" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="1">
-        <v>855000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15">
-      <c r="G17" s="17"/>
-      <c r="M17" s="11"/>
-      <c r="O17" s="20">
-        <f>SUM(O15:O16)</f>
-        <v>1105720</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15">
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="P15" s="10"/>
+      <c r="R15" s="2">
+        <f>SUM(R3:R14)</f>
+        <v>257050</v>
+      </c>
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="16"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="16"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="4"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="1">
+        <v>240000</v>
+      </c>
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="C17" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="16"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="16"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="4"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="1">
+        <v>110000</v>
+      </c>
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="C18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="16"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="16"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="4"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18" s="1">
+        <v>180000</v>
+      </c>
+      <c r="S18" s="10"/>
+    </row>
+    <row r="19" spans="2:19">
+      <c r="G19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="M19" s="4"/>
+      <c r="O19" s="18">
+        <f>SUM(O14:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="11"/>
+      <c r="Q19" t="s">
+        <v>47</v>
+      </c>
+      <c r="R19" s="1">
+        <v>68000</v>
+      </c>
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="2:19">
+      <c r="G20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="P20" s="11"/>
+      <c r="R20" s="20">
+        <f>SUM(R15:R19)</f>
+        <v>855050</v>
+      </c>
+      <c r="S20" s="11"/>
+    </row>
+    <row r="24" spans="2:19">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F3:F12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>F3-E3 &lt;&gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1"/>
-    <hyperlink ref="C23" r:id="rId2"/>
+    <hyperlink ref="C24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1372,11 +1641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1394,44 +1663,51 @@
     <col min="12" max="12" width="4.25" customWidth="1"/>
     <col min="14" max="14" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.25" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.125" style="1" customWidth="1"/>
     <col min="18" max="18" width="4.25" customWidth="1"/>
-    <col min="20" max="20" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="4.25" customWidth="1"/>
+    <col min="23" max="23" width="10.875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23" ht="36" customHeight="1">
       <c r="C1" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="23"/>
       <c r="G1" s="33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="15"/>
       <c r="J1" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="27"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="32"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="L1" s="12"/>
+      <c r="M1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="32"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="29"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="32"/>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1439,56 +1715,63 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="9"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="12"/>
+      <c r="R2" s="9"/>
       <c r="S2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="12"/>
+      <c r="V2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <v>138500</v>
@@ -1516,7 +1799,7 @@
         <f>$C3*J3</f>
         <v>138500</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="13"/>
       <c r="M3">
         <v>0</v>
       </c>
@@ -1524,7 +1807,7 @@
         <f>$C3*M3</f>
         <v>0</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="5"/>
       <c r="P3">
         <v>0</v>
       </c>
@@ -1532,7 +1815,7 @@
         <f>$C3*P3</f>
         <v>0</v>
       </c>
-      <c r="R3" s="13"/>
+      <c r="R3" s="10"/>
       <c r="S3">
         <v>0</v>
       </c>
@@ -1540,13 +1823,21 @@
         <f>$C3*S3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="13"/>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <f>$C3*V3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>24850</v>
@@ -1574,15 +1865,15 @@
         <f t="shared" ref="K4:K13" si="2">$C4*J4</f>
         <v>24850</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="13"/>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" ref="N4:N13" si="3">$C4*M4</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="10"/>
+        <v>24850</v>
+      </c>
+      <c r="O4" s="5"/>
       <c r="P4">
         <v>0</v>
       </c>
@@ -1590,7 +1881,7 @@
         <f t="shared" ref="Q4:Q13" si="4">$C4*P4</f>
         <v>0</v>
       </c>
-      <c r="R4" s="13"/>
+      <c r="R4" s="10"/>
       <c r="S4">
         <v>0</v>
       </c>
@@ -1598,13 +1889,21 @@
         <f t="shared" ref="T4:T13" si="5">$C4*S4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="13"/>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" ref="W4:W13" si="6">$C4*V4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1">
         <v>112100</v>
@@ -1632,7 +1931,7 @@
         <f t="shared" si="2"/>
         <v>112100</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="13"/>
       <c r="M5">
         <v>0</v>
       </c>
@@ -1640,7 +1939,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O5" s="10"/>
+      <c r="O5" s="5"/>
       <c r="P5">
         <v>0</v>
       </c>
@@ -1648,7 +1947,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R5" s="13"/>
+      <c r="R5" s="10"/>
       <c r="S5">
         <v>0</v>
       </c>
@@ -1656,13 +1955,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" s="13"/>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>45340</v>
@@ -1690,15 +1997,15 @@
         <f t="shared" si="2"/>
         <v>181360</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="13"/>
       <c r="M6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="3"/>
-        <v>90680</v>
-      </c>
-      <c r="O6" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="5"/>
       <c r="P6">
         <v>2</v>
       </c>
@@ -1706,7 +2013,7 @@
         <f t="shared" si="4"/>
         <v>90680</v>
       </c>
-      <c r="R6" s="13"/>
+      <c r="R6" s="10"/>
       <c r="S6">
         <v>0</v>
       </c>
@@ -1714,13 +2021,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="13"/>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>137500</v>
@@ -1742,13 +2057,13 @@
       </c>
       <c r="I7" s="16"/>
       <c r="J7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>275000</v>
-      </c>
-      <c r="L7" s="5"/>
+        <v>137500</v>
+      </c>
+      <c r="L7" s="13"/>
       <c r="M7">
         <v>1</v>
       </c>
@@ -1756,15 +2071,15 @@
         <f t="shared" si="3"/>
         <v>137500</v>
       </c>
-      <c r="O7" s="10"/>
+      <c r="O7" s="5"/>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="13"/>
+        <v>137500</v>
+      </c>
+      <c r="R7" s="10"/>
       <c r="S7">
         <v>0</v>
       </c>
@@ -1772,13 +2087,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" s="13"/>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>79600</v>
@@ -1806,15 +2129,15 @@
         <f t="shared" si="2"/>
         <v>79600</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="13"/>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="10"/>
+        <v>79600</v>
+      </c>
+      <c r="O8" s="5"/>
       <c r="P8">
         <v>0</v>
       </c>
@@ -1822,7 +2145,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R8" s="13"/>
+      <c r="R8" s="10"/>
       <c r="S8">
         <v>0</v>
       </c>
@@ -1830,13 +2153,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" s="13"/>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>51000</v>
@@ -1864,15 +2195,15 @@
         <f t="shared" si="2"/>
         <v>51000</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="13"/>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="10"/>
+        <v>51000</v>
+      </c>
+      <c r="O9" s="5"/>
       <c r="P9">
         <v>0</v>
       </c>
@@ -1880,7 +2211,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R9" s="13"/>
+      <c r="R9" s="10"/>
       <c r="S9">
         <v>0</v>
       </c>
@@ -1888,13 +2219,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9" s="13"/>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>11300</v>
@@ -1916,21 +2255,21 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>22600</v>
-      </c>
-      <c r="L10" s="5"/>
+        <v>11300</v>
+      </c>
+      <c r="L10" s="13"/>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="10"/>
+        <v>11300</v>
+      </c>
+      <c r="O10" s="5"/>
       <c r="P10">
         <v>0</v>
       </c>
@@ -1938,7 +2277,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R10" s="13"/>
+      <c r="R10" s="10"/>
       <c r="S10">
         <v>0</v>
       </c>
@@ -1946,13 +2285,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="13"/>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>258000</v>
@@ -1980,32 +2327,40 @@
         <f t="shared" si="2"/>
         <v>258000</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="13"/>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="10"/>
+        <v>258000</v>
+      </c>
+      <c r="O11" s="5"/>
       <c r="P11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="4"/>
-        <v>258000</v>
-      </c>
-      <c r="R11" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="10"/>
       <c r="S11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="13"/>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" si="6"/>
         <v>258000</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:23">
       <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2020,23 +2375,28 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="13"/>
       <c r="N12" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O12" s="10"/>
+      <c r="O12" s="5"/>
       <c r="Q12" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R12" s="13"/>
+      <c r="R12" s="10"/>
       <c r="T12" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" s="13"/>
+      <c r="W12" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2051,25 +2411,30 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L13" s="4"/>
+      <c r="L13" s="14"/>
       <c r="N13" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O13" s="11"/>
+      <c r="O13" s="4"/>
       <c r="Q13" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R13" s="14"/>
+      <c r="R13" s="11"/>
       <c r="T13" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13" s="14"/>
+      <c r="W13" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2">
         <f>SUM(E3:E13)</f>
@@ -2083,76 +2448,94 @@
       <c r="I14" s="16"/>
       <c r="K14" s="2">
         <f>SUM(K3:K13)</f>
-        <v>1143010</v>
-      </c>
-      <c r="L14" s="5"/>
+        <v>994210</v>
+      </c>
+      <c r="L14" s="13"/>
       <c r="N14" s="1">
         <f>SUM(N3:N13)</f>
-        <v>228180</v>
-      </c>
-      <c r="O14" s="10"/>
+        <v>562250</v>
+      </c>
+      <c r="O14" s="5"/>
       <c r="Q14" s="1">
         <f>SUM(Q3:Q13)</f>
-        <v>348680</v>
-      </c>
-      <c r="R14" s="13"/>
+        <v>228180</v>
+      </c>
+      <c r="R14" s="10"/>
       <c r="T14" s="1">
         <f>SUM(T3:T13)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="13"/>
+      <c r="W14" s="1">
+        <f>SUM(W3:W13)</f>
         <v>258000</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:23">
       <c r="F15" s="25"/>
       <c r="I15" s="17"/>
-      <c r="L15" s="4"/>
+      <c r="L15" s="14"/>
       <c r="M15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N15" s="1">
+        <v>420000</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="1">
         <v>530000</v>
       </c>
-      <c r="O15" s="11"/>
-      <c r="P15" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>500000</v>
-      </c>
-      <c r="R15" s="14"/>
+      <c r="R15" s="11"/>
       <c r="S15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15" s="1">
+        <v>760000</v>
+      </c>
+      <c r="U15" s="14"/>
+      <c r="V15" t="s">
+        <v>26</v>
+      </c>
+      <c r="W15" s="1">
         <v>560000</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:23">
       <c r="F16" s="25"/>
       <c r="I16" s="17"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="14"/>
       <c r="N16" s="18">
         <f>SUM(N14:N15)</f>
+        <v>982250</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="Q16" s="18">
+        <f>SUM(Q14:Q15)</f>
         <v>758180</v>
       </c>
-      <c r="O16" s="11"/>
-      <c r="Q16" s="20">
-        <f>SUM(Q14:Q15)</f>
-        <v>848680</v>
-      </c>
-      <c r="R16" s="14"/>
-      <c r="T16" s="19">
+      <c r="R16" s="11"/>
+      <c r="T16" s="20">
         <f>SUM(T14:T15)</f>
+        <v>760000</v>
+      </c>
+      <c r="U16" s="14"/>
+      <c r="W16" s="19">
+        <f>SUM(W14:W15)</f>
         <v>818000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>